<commit_message>
23.06.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/June/Others/Allocation Sheet.xlsx
+++ b/June/Others/Allocation Sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="99">
   <si>
     <t>BL60</t>
   </si>
@@ -25,9 +25,6 @@
     <t>B17</t>
   </si>
   <si>
-    <t>T200</t>
-  </si>
-  <si>
     <t>BL90</t>
   </si>
   <si>
@@ -136,21 +133,12 @@
     <t>T130</t>
   </si>
   <si>
-    <t>E90</t>
-  </si>
-  <si>
-    <t>L65j</t>
-  </si>
-  <si>
     <t>L52</t>
   </si>
   <si>
     <t>B17i</t>
   </si>
   <si>
-    <t>i90</t>
-  </si>
-  <si>
     <t>L60</t>
   </si>
   <si>
@@ -172,24 +160,15 @@
     <t>V78</t>
   </si>
   <si>
-    <t>V94</t>
-  </si>
-  <si>
     <t>D54j</t>
   </si>
   <si>
     <t>D38</t>
   </si>
   <si>
-    <t>D75</t>
-  </si>
-  <si>
     <t>i95</t>
   </si>
   <si>
-    <t>L200</t>
-  </si>
-  <si>
     <t>V142</t>
   </si>
   <si>
@@ -199,21 +178,12 @@
     <t>BL70</t>
   </si>
   <si>
-    <t>L120</t>
-  </si>
-  <si>
-    <t>L150</t>
-  </si>
-  <si>
     <t>V75m</t>
   </si>
   <si>
     <t>V97</t>
   </si>
   <si>
-    <t>Z10</t>
-  </si>
-  <si>
     <t>P11</t>
   </si>
   <si>
@@ -277,21 +247,6 @@
     <t>L100</t>
   </si>
   <si>
-    <t>L300</t>
-  </si>
-  <si>
-    <t>i10+skd</t>
-  </si>
-  <si>
-    <t>i110skd</t>
-  </si>
-  <si>
-    <t>S10</t>
-  </si>
-  <si>
-    <t>S5</t>
-  </si>
-  <si>
     <t>V120</t>
   </si>
   <si>
@@ -304,21 +259,9 @@
     <t>V48_SKD</t>
   </si>
   <si>
-    <t>V75m_2GB</t>
-  </si>
-  <si>
-    <t>V75skd</t>
-  </si>
-  <si>
     <t>V90</t>
   </si>
   <si>
-    <t>V98skd</t>
-  </si>
-  <si>
-    <t>P8 Pro</t>
-  </si>
-  <si>
     <t>Issue</t>
   </si>
   <si>
@@ -340,7 +283,34 @@
     <t>Office:01715-116767</t>
   </si>
   <si>
-    <t>Shohel: 01774-585840</t>
+    <t>i18</t>
+  </si>
+  <si>
+    <t>L65j_SKD</t>
+  </si>
+  <si>
+    <t>E90_SKD</t>
+  </si>
+  <si>
+    <t>i10+_skd</t>
+  </si>
+  <si>
+    <t>i110_skd</t>
+  </si>
+  <si>
+    <t>V75_skd</t>
+  </si>
+  <si>
+    <t>V94_skd</t>
+  </si>
+  <si>
+    <t>V98_skd</t>
+  </si>
+  <si>
+    <t>Robiul : 01751-312831</t>
+  </si>
+  <si>
+    <t>B60</t>
   </si>
 </sst>
 </file>
@@ -608,69 +578,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -687,6 +606,57 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 2" xfId="1"/>
@@ -1084,90 +1054,90 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="45" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="45"/>
-    <col min="3" max="4" width="8.140625" style="45" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="45" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="45" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="45" customWidth="1"/>
-    <col min="8" max="8" width="1.85546875" style="45" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="45" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="45" customWidth="1"/>
-    <col min="11" max="12" width="7.140625" style="45" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="45" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="45" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" style="45" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="45"/>
+    <col min="1" max="1" width="7.5703125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="28"/>
+    <col min="3" max="4" width="8.140625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="28" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" style="28" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="28" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" style="28" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="28" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="28" customWidth="1"/>
+    <col min="11" max="12" width="7.140625" style="28" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" style="28" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="28" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="28" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="32.25" customHeight="1">
-      <c r="A1" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="A1" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-    </row>
-    <row r="3" spans="1:18" s="46" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
+      <c r="A2" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+    </row>
+    <row r="3" spans="1:18" s="29" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A3" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
     </row>
     <row r="4" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
+      <c r="A4" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
@@ -1175,61 +1145,61 @@
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
-      <c r="L4" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
+      <c r="L4" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickTop="1">
       <c r="A5" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="E5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="G5" s="9" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="M5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="O5" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.95" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B6" s="6">
         <v>800</v>
@@ -1243,13 +1213,13 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="13" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="J6" s="4">
-        <v>7490</v>
+        <v>4640</v>
       </c>
       <c r="K6" s="3">
-        <v>7990</v>
+        <v>4990</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -1272,23 +1242,23 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" s="36">
-        <v>9190</v>
+        <v>15</v>
+      </c>
+      <c r="J7" s="21">
+        <v>5650</v>
       </c>
       <c r="K7" s="3">
-        <v>9990</v>
+        <v>6150</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="R7" s="47"/>
+      <c r="R7" s="30"/>
     </row>
     <row r="8" spans="1:18" ht="15.95" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B8" s="6">
         <v>810</v>
@@ -1302,13 +1272,13 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="2" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="J8" s="2">
-        <v>5750</v>
+        <v>5020</v>
       </c>
       <c r="K8" s="3">
-        <v>6190</v>
+        <v>5390</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1317,7 +1287,7 @@
     </row>
     <row r="9" spans="1:18" ht="15.95" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B9" s="6">
         <v>800</v>
@@ -1331,13 +1301,13 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="2" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="J9" s="4">
-        <v>17790</v>
+        <v>5280</v>
       </c>
       <c r="K9" s="3">
-        <v>18990</v>
+        <v>5690</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -1346,7 +1316,7 @@
     </row>
     <row r="10" spans="1:18" ht="15.95" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="6">
         <v>795</v>
@@ -1360,13 +1330,13 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="14" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="J10" s="4">
-        <v>10330</v>
+        <v>5100</v>
       </c>
       <c r="K10" s="3">
-        <v>10990</v>
+        <v>5490</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -1375,7 +1345,7 @@
     </row>
     <row r="11" spans="1:18" ht="15.95" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="6">
         <v>790</v>
@@ -1389,10 +1359,10 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="14" t="s">
-        <v>92</v>
+        <v>34</v>
       </c>
       <c r="J11" s="4">
-        <v>5570</v>
+        <v>5560</v>
       </c>
       <c r="K11" s="3">
         <v>5990</v>
@@ -1404,13 +1374,13 @@
     </row>
     <row r="12" spans="1:18" ht="15.95" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="B12" s="6">
-        <v>970</v>
+        <v>800</v>
       </c>
       <c r="C12" s="3">
-        <v>1060</v>
+        <v>860</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1418,13 +1388,13 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="2" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="J12" s="4">
-        <v>4640</v>
+        <v>6090</v>
       </c>
       <c r="K12" s="3">
-        <v>4990</v>
+        <v>6590</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -1433,13 +1403,13 @@
     </row>
     <row r="13" spans="1:18" ht="15.95" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B13" s="6">
-        <v>900</v>
+        <v>970</v>
       </c>
       <c r="C13" s="3">
-        <v>975</v>
+        <v>1060</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1447,13 +1417,13 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="13" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="J13" s="4">
-        <v>5650</v>
+        <v>5390</v>
       </c>
       <c r="K13" s="3">
-        <v>6150</v>
+        <v>5790</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -1462,13 +1432,13 @@
     </row>
     <row r="14" spans="1:18" ht="15.95" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="B14" s="6">
-        <v>915</v>
+        <v>900</v>
       </c>
       <c r="C14" s="3">
-        <v>990</v>
+        <v>975</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1476,13 +1446,13 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="2" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="J14" s="4">
-        <v>5020</v>
+        <v>3630</v>
       </c>
       <c r="K14" s="3">
-        <v>5390</v>
+        <v>3890</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -1491,13 +1461,13 @@
     </row>
     <row r="15" spans="1:18" ht="15.95" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="B15" s="6">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="C15" s="3">
-        <v>980</v>
+        <v>990</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1505,13 +1475,13 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="13" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="J15" s="4">
-        <v>5280</v>
+        <v>3560</v>
       </c>
       <c r="K15" s="3">
-        <v>5690</v>
+        <v>3840</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
@@ -1520,13 +1490,13 @@
     </row>
     <row r="16" spans="1:18" ht="15.95" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="B16" s="6">
-        <v>890</v>
+        <v>910</v>
       </c>
       <c r="C16" s="3">
-        <v>970</v>
+        <v>980</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -1534,13 +1504,13 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="13" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="J16" s="4">
-        <v>5100</v>
+        <v>3340</v>
       </c>
       <c r="K16" s="3">
-        <v>5490</v>
+        <v>3590</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -1549,13 +1519,13 @@
     </row>
     <row r="17" spans="1:15" ht="15.95" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B17" s="6">
-        <v>920</v>
+        <v>890</v>
       </c>
       <c r="C17" s="3">
-        <v>999</v>
+        <v>970</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -1563,13 +1533,13 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="2" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="J17" s="4">
-        <v>5560</v>
+        <v>5390</v>
       </c>
       <c r="K17" s="3">
-        <v>5990</v>
+        <v>5790</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -1578,13 +1548,13 @@
     </row>
     <row r="18" spans="1:15" ht="15.95" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="B18" s="6">
-        <v>880</v>
+        <v>920</v>
       </c>
       <c r="C18" s="3">
-        <v>950</v>
+        <v>999</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1592,13 +1562,13 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="2" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="J18" s="4">
-        <v>6090</v>
+        <v>4500</v>
       </c>
       <c r="K18" s="3">
-        <v>6590</v>
+        <v>4790</v>
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -1607,13 +1577,13 @@
     </row>
     <row r="19" spans="1:15" ht="15.95" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B19" s="6">
-        <v>1000</v>
+        <v>880</v>
       </c>
       <c r="C19" s="3">
-        <v>1090</v>
+        <v>950</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1621,13 +1591,13 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="13" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J19" s="4">
-        <v>5390</v>
+        <v>4970</v>
       </c>
       <c r="K19" s="3">
-        <v>5790</v>
+        <v>5290</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
@@ -1636,13 +1606,13 @@
     </row>
     <row r="20" spans="1:15" ht="15.95" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B20" s="6">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="C20" s="3">
-        <v>1075</v>
+        <v>1090</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1650,13 +1620,13 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="J20" s="4">
-        <v>3630</v>
+        <v>4015</v>
       </c>
       <c r="K20" s="3">
-        <v>3890</v>
+        <v>4390</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -1665,13 +1635,13 @@
     </row>
     <row r="21" spans="1:15" ht="15.95" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="B21" s="6">
-        <v>1000</v>
+        <v>995</v>
       </c>
       <c r="C21" s="3">
-        <v>1090</v>
+        <v>1075</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -1679,13 +1649,13 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="J21" s="4">
-        <v>3560</v>
+        <v>3710</v>
       </c>
       <c r="K21" s="3">
-        <v>3840</v>
+        <v>3990</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -1694,13 +1664,13 @@
     </row>
     <row r="22" spans="1:15" ht="15.95" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" s="6">
-        <v>960</v>
+        <v>1000</v>
       </c>
       <c r="C22" s="3">
-        <v>1040</v>
+        <v>1090</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1711,10 +1681,10 @@
         <v>95</v>
       </c>
       <c r="J22" s="4">
-        <v>3340</v>
+        <v>3620</v>
       </c>
       <c r="K22" s="3">
-        <v>3590</v>
+        <v>3890</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -1723,13 +1693,13 @@
     </row>
     <row r="23" spans="1:15" ht="15.95" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" s="6">
+        <v>960</v>
+      </c>
+      <c r="C23" s="3">
         <v>1040</v>
-      </c>
-      <c r="C23" s="3">
-        <v>1120</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -1737,13 +1707,13 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="2" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J23" s="4">
-        <v>5390</v>
+        <v>4620</v>
       </c>
       <c r="K23" s="3">
-        <v>5790</v>
+        <v>4999</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -1752,13 +1722,13 @@
     </row>
     <row r="24" spans="1:15" ht="15.95" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="B24" s="6">
-        <v>1290</v>
+        <v>1040</v>
       </c>
       <c r="C24" s="3">
-        <v>1390</v>
+        <v>1120</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1766,13 +1736,13 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="2" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="J24" s="4">
-        <v>5740</v>
+        <v>4520</v>
       </c>
       <c r="K24" s="3">
-        <v>6190</v>
+        <v>4899</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -1781,13 +1751,13 @@
     </row>
     <row r="25" spans="1:15" ht="15.95" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B25" s="6">
-        <v>1190</v>
+        <v>1290</v>
       </c>
       <c r="C25" s="3">
-        <v>1290</v>
+        <v>1390</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1795,13 +1765,13 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="2" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="J25" s="4">
-        <v>4500</v>
+        <v>4080</v>
       </c>
       <c r="K25" s="3">
-        <v>4790</v>
+        <v>4390</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
@@ -1810,13 +1780,13 @@
     </row>
     <row r="26" spans="1:15" ht="15.95" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="B26" s="6">
-        <v>1270</v>
+        <v>1190</v>
       </c>
       <c r="C26" s="3">
-        <v>1370</v>
+        <v>1290</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1824,13 +1794,13 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="2" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="J26" s="4">
-        <v>4970</v>
+        <v>4220</v>
       </c>
       <c r="K26" s="3">
-        <v>5290</v>
+        <v>4540</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
@@ -1839,13 +1809,13 @@
     </row>
     <row r="27" spans="1:15" ht="15.95" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="B27" s="6">
-        <v>1170</v>
+        <v>1270</v>
       </c>
       <c r="C27" s="3">
-        <v>1270</v>
+        <v>1370</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1853,13 +1823,13 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="2" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="J27" s="4">
-        <v>4015</v>
+        <v>12240</v>
       </c>
       <c r="K27" s="3">
-        <v>4390</v>
+        <v>12990</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -1868,13 +1838,13 @@
     </row>
     <row r="28" spans="1:15" ht="15.95" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="B28" s="6">
-        <v>1190</v>
+        <v>1170</v>
       </c>
       <c r="C28" s="3">
-        <v>1290</v>
+        <v>1270</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1882,13 +1852,13 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="14" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J28" s="4">
-        <v>3710</v>
+        <v>12090</v>
       </c>
       <c r="K28" s="3">
-        <v>3890</v>
+        <v>12990</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -1897,13 +1867,13 @@
     </row>
     <row r="29" spans="1:15" ht="15.95" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="B29" s="6">
+        <v>1190</v>
+      </c>
+      <c r="C29" s="3">
         <v>1290</v>
-      </c>
-      <c r="C29" s="3">
-        <v>1390</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1911,13 +1881,13 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="14" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="J29" s="4">
-        <v>3620</v>
+        <v>10840</v>
       </c>
       <c r="K29" s="3">
-        <v>4290</v>
+        <v>11990</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
@@ -1926,7 +1896,7 @@
     </row>
     <row r="30" spans="1:15" ht="15.95" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B30" s="6">
         <v>1225</v>
@@ -1940,13 +1910,13 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J30" s="36">
-        <v>4620</v>
+        <v>59</v>
+      </c>
+      <c r="J30" s="21">
+        <v>12490</v>
       </c>
       <c r="K30" s="3">
-        <v>4999</v>
+        <v>13490</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -1955,7 +1925,7 @@
     </row>
     <row r="31" spans="1:15" ht="15.95" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="6">
         <v>1220</v>
@@ -1969,13 +1939,13 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J31" s="36">
-        <v>4520</v>
+        <v>84</v>
+      </c>
+      <c r="J31" s="21">
+        <v>8820</v>
       </c>
       <c r="K31" s="3">
-        <v>4899</v>
+        <v>9490</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -1984,28 +1954,22 @@
     </row>
     <row r="32" spans="1:15" ht="15.95" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="B32" s="6">
-        <v>1460</v>
+        <v>1080</v>
       </c>
       <c r="C32" s="3">
-        <v>1590</v>
+        <v>1160</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J32" s="36">
-        <v>4080</v>
-      </c>
-      <c r="K32" s="3">
-        <v>4390</v>
-      </c>
+      <c r="I32" s="13"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
@@ -2013,28 +1977,22 @@
     </row>
     <row r="33" spans="1:15" ht="15.95" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B33" s="6">
-        <v>1470</v>
+        <v>1100</v>
       </c>
       <c r="C33" s="3">
-        <v>1590</v>
+        <v>1199</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="J33" s="4">
-        <v>4220</v>
-      </c>
-      <c r="K33" s="3">
-        <v>4540</v>
-      </c>
+      <c r="I33" s="13"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
@@ -2042,28 +2000,22 @@
     </row>
     <row r="34" spans="1:15" ht="15.95" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B34" s="6">
-        <v>1590</v>
+        <v>1200</v>
       </c>
       <c r="C34" s="3">
-        <v>1740</v>
+        <v>1290</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J34" s="36">
-        <v>12590</v>
-      </c>
-      <c r="K34" s="3">
-        <v>13490</v>
-      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
@@ -2071,28 +2023,22 @@
     </row>
     <row r="35" spans="1:15" ht="15.95" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B35" s="6">
-        <v>1080</v>
+        <v>1120</v>
       </c>
       <c r="C35" s="3">
-        <v>1160</v>
+        <v>1220</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
-      <c r="I35" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J35" s="4">
-        <v>12240</v>
-      </c>
-      <c r="K35" s="3">
-        <v>12990</v>
-      </c>
+      <c r="I35" s="2"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
@@ -2100,28 +2046,22 @@
     </row>
     <row r="36" spans="1:15" ht="15.95" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B36" s="7">
-        <v>1100</v>
+        <v>1040</v>
       </c>
       <c r="C36" s="3">
-        <v>1199</v>
+        <v>1130</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="J36" s="4">
-        <v>8270</v>
-      </c>
-      <c r="K36" s="3">
-        <v>8990</v>
-      </c>
+      <c r="I36" s="13"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
@@ -2129,28 +2069,22 @@
     </row>
     <row r="37" spans="1:15" ht="15.95" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="B37" s="6">
-        <v>1200</v>
+        <v>1100</v>
       </c>
       <c r="C37" s="3">
-        <v>1290</v>
+        <v>1199</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="J37" s="4">
-        <v>12090</v>
-      </c>
-      <c r="K37" s="3">
-        <v>12990</v>
-      </c>
+      <c r="I37" s="13"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
@@ -2158,28 +2092,22 @@
     </row>
     <row r="38" spans="1:15" ht="15.95" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B38" s="6">
-        <v>1120</v>
+        <v>1100</v>
       </c>
       <c r="C38" s="3">
-        <v>1220</v>
+        <v>1199</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J38" s="4">
-        <v>10840</v>
-      </c>
-      <c r="K38" s="3">
-        <v>11990</v>
-      </c>
+      <c r="I38" s="13"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
@@ -2187,28 +2115,22 @@
     </row>
     <row r="39" spans="1:15" ht="15.95" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="B39" s="6">
-        <v>1730</v>
+        <v>1050</v>
       </c>
       <c r="C39" s="3">
-        <v>1890</v>
+        <v>1130</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="I39" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="J39" s="4">
-        <v>12490</v>
-      </c>
-      <c r="K39" s="3">
-        <v>13490</v>
-      </c>
+      <c r="I39" s="13"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
@@ -2216,28 +2138,22 @@
     </row>
     <row r="40" spans="1:15" ht="15.95" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B40" s="6">
-        <v>1040</v>
+        <v>1130</v>
       </c>
       <c r="C40" s="3">
-        <v>1130</v>
+        <v>1230</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-      <c r="I40" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="J40" s="36">
-        <v>8820</v>
-      </c>
-      <c r="K40" s="3">
-        <v>9490</v>
-      </c>
+      <c r="I40" s="3"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
@@ -2245,28 +2161,22 @@
     </row>
     <row r="41" spans="1:15" ht="15.95" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B41" s="6">
         <v>1100</v>
       </c>
       <c r="C41" s="3">
-        <v>1199</v>
+        <v>1190</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J41" s="4">
-        <v>5940</v>
-      </c>
-      <c r="K41" s="3">
-        <v>6390</v>
-      </c>
+      <c r="I41" s="14"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -2274,13 +2184,13 @@
     </row>
     <row r="42" spans="1:15" ht="15.95" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="B42" s="6">
-        <v>1100</v>
+        <v>1330</v>
       </c>
       <c r="C42" s="3">
-        <v>1199</v>
+        <v>1450</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -2297,13 +2207,13 @@
     </row>
     <row r="43" spans="1:15" ht="15.95" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="B43" s="6">
-        <v>1050</v>
+        <v>1200</v>
       </c>
       <c r="C43" s="3">
-        <v>1130</v>
+        <v>1299</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -2320,122 +2230,122 @@
     </row>
     <row r="44" spans="1:15" ht="15.95" customHeight="1">
       <c r="A44" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B44" s="6">
-        <v>1130</v>
+        <v>1250</v>
       </c>
       <c r="C44" s="3">
-        <v>1230</v>
+        <v>1350</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="I44" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="J44" s="24"/>
-      <c r="K44" s="38"/>
-      <c r="L44" s="38"/>
-      <c r="M44" s="37"/>
-      <c r="N44" s="37"/>
+      <c r="I44" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J44" s="36"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="35"/>
+      <c r="N44" s="35"/>
       <c r="O44" s="12"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B45" s="6">
-        <v>1100</v>
+        <v>1370</v>
       </c>
       <c r="C45" s="3">
-        <v>1190</v>
+        <v>1490</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37"/>
-      <c r="K45" s="37"/>
-      <c r="L45" s="37"/>
-      <c r="M45" s="37"/>
-      <c r="N45" s="37"/>
-      <c r="O45" s="37"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="35"/>
+      <c r="M45" s="35"/>
+      <c r="N45" s="35"/>
+      <c r="O45" s="35"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="B46" s="6">
-        <v>1330</v>
+        <v>2780</v>
       </c>
       <c r="C46" s="3">
-        <v>1450</v>
+        <v>2990</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-      <c r="I46" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="J46" s="39"/>
-      <c r="K46" s="39"/>
-      <c r="L46" s="39"/>
-      <c r="M46" s="39"/>
-      <c r="N46" s="39"/>
-      <c r="O46" s="31"/>
+      <c r="I46" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="J46" s="43"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="43"/>
+      <c r="M46" s="43"/>
+      <c r="N46" s="43"/>
+      <c r="O46" s="44"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="B47" s="6">
-        <v>1200</v>
+        <v>6540</v>
       </c>
       <c r="C47" s="3">
-        <v>1299</v>
+        <v>6990</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
-      <c r="I47" s="19" t="s">
-        <v>70</v>
+      <c r="I47" s="20" t="s">
+        <v>60</v>
       </c>
       <c r="J47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K47" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="K47" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="L47" s="34"/>
-      <c r="M47" s="34"/>
-      <c r="N47" s="34"/>
-      <c r="O47" s="32"/>
+      <c r="L47" s="47"/>
+      <c r="M47" s="47"/>
+      <c r="N47" s="47"/>
+      <c r="O47" s="45"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B48" s="6">
-        <v>1250</v>
+        <v>5290</v>
       </c>
       <c r="C48" s="3">
-        <v>1350</v>
+        <v>5690</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
-      <c r="I48" s="19">
+      <c r="I48" s="20">
         <v>1000</v>
       </c>
       <c r="J48" s="5"/>
@@ -2443,24 +2353,24 @@
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
-      <c r="O48" s="32"/>
+      <c r="O48" s="45"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="B49" s="6">
-        <v>1370</v>
+        <v>5470</v>
       </c>
       <c r="C49" s="3">
-        <v>1470</v>
+        <v>5890</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="19">
+      <c r="I49" s="20">
         <v>500</v>
       </c>
       <c r="J49" s="5"/>
@@ -2468,24 +2378,24 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
-      <c r="O49" s="32"/>
+      <c r="O49" s="45"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="B50" s="3">
-        <v>1890</v>
+        <v>5750</v>
       </c>
       <c r="C50" s="3">
-        <v>2090</v>
+        <v>6190</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
-      <c r="I50" s="19">
+      <c r="I50" s="20">
         <v>100</v>
       </c>
       <c r="J50" s="5"/>
@@ -2493,24 +2403,24 @@
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
-      <c r="O50" s="32"/>
+      <c r="O50" s="45"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="B51" s="3">
-        <v>2780</v>
+        <v>5940</v>
       </c>
       <c r="C51" s="3">
-        <v>2990</v>
+        <v>6390</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
-      <c r="I51" s="19">
+      <c r="I51" s="20">
         <v>50</v>
       </c>
       <c r="J51" s="5"/>
@@ -2518,24 +2428,24 @@
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
-      <c r="O51" s="32"/>
+      <c r="O51" s="45"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B52" s="3">
-        <v>5290</v>
+        <v>6530</v>
       </c>
       <c r="C52" s="3">
-        <v>5690</v>
+        <v>6990</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
-      <c r="I52" s="19">
+      <c r="I52" s="20">
         <v>20</v>
       </c>
       <c r="J52" s="5"/>
@@ -2543,24 +2453,24 @@
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
-      <c r="O52" s="32"/>
+      <c r="O52" s="45"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B53" s="3">
-        <v>5750</v>
+        <v>8340</v>
       </c>
       <c r="C53" s="3">
-        <v>6190</v>
+        <v>8990</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="19">
+      <c r="I53" s="20">
         <v>10</v>
       </c>
       <c r="J53" s="5"/>
@@ -2568,24 +2478,24 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
-      <c r="O53" s="32"/>
+      <c r="O53" s="45"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="B54" s="3">
-        <v>6540</v>
+        <v>9190</v>
       </c>
       <c r="C54" s="3">
-        <v>6990</v>
+        <v>9990</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="19">
+      <c r="I54" s="20">
         <v>5</v>
       </c>
       <c r="J54" s="5"/>
@@ -2593,24 +2503,24 @@
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
-      <c r="O54" s="32"/>
+      <c r="O54" s="45"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="B55" s="3">
-        <v>8340</v>
+        <v>5750</v>
       </c>
       <c r="C55" s="3">
-        <v>8990</v>
+        <v>6190</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
-      <c r="I55" s="19">
+      <c r="I55" s="20">
         <v>2</v>
       </c>
       <c r="J55" s="5"/>
@@ -2618,17 +2528,17 @@
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
-      <c r="O55" s="32"/>
+      <c r="O55" s="45"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="2" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="B56" s="2">
-        <v>7890</v>
+        <v>5570</v>
       </c>
       <c r="C56" s="2">
-        <v>8290</v>
+        <v>5990</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -2636,105 +2546,105 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
-      <c r="O56" s="33"/>
+      <c r="O56" s="46"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="11"/>
       <c r="B57" s="1"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
       <c r="E57" s="11"/>
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
       <c r="I57" s="11"/>
-      <c r="J57" s="40"/>
-      <c r="K57" s="20"/>
-      <c r="L57" s="20"/>
-      <c r="M57" s="41"/>
-      <c r="N57" s="41"/>
-      <c r="O57" s="41"/>
+      <c r="J57" s="23"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18"/>
+      <c r="M57" s="24"/>
+      <c r="N57" s="24"/>
+      <c r="O57" s="24"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B58" s="29"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="42"/>
-      <c r="F58" s="42"/>
-      <c r="G58" s="42"/>
-      <c r="H58" s="42"/>
-      <c r="I58" s="42"/>
-      <c r="J58" s="43"/>
-      <c r="K58" s="18"/>
-      <c r="L58" s="18"/>
-      <c r="M58" s="42"/>
-      <c r="N58" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="O58" s="30"/>
+      <c r="A58" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" s="41"/>
+      <c r="C58" s="41"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="25"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="19"/>
+      <c r="L58" s="19"/>
+      <c r="M58" s="25"/>
+      <c r="N58" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="O58" s="42"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="23"/>
-      <c r="B59" s="23"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="20"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="18"/>
       <c r="E59" s="11"/>
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
       <c r="I59" s="11"/>
-      <c r="J59" s="40"/>
-      <c r="K59" s="20"/>
-      <c r="L59" s="20"/>
+      <c r="J59" s="23"/>
+      <c r="K59" s="18"/>
+      <c r="L59" s="18"/>
       <c r="M59" s="11"/>
-      <c r="N59" s="23"/>
-      <c r="O59" s="23"/>
+      <c r="N59" s="34"/>
+      <c r="O59" s="34"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="23"/>
-      <c r="B60" s="23"/>
-      <c r="C60" s="23"/>
-      <c r="D60" s="20"/>
+      <c r="A60" s="34"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="18"/>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
       <c r="I60" s="11"/>
-      <c r="J60" s="40"/>
-      <c r="K60" s="20"/>
-      <c r="L60" s="20"/>
+      <c r="J60" s="23"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="18"/>
       <c r="M60" s="11"/>
-      <c r="N60" s="23"/>
-      <c r="O60" s="23"/>
+      <c r="N60" s="34"/>
+      <c r="O60" s="34"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B61" s="29"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="18"/>
-      <c r="I61" s="18"/>
-      <c r="J61" s="44"/>
-      <c r="K61" s="18"/>
-      <c r="L61" s="18"/>
+      <c r="A61" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="41"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="27"/>
+      <c r="K61" s="19"/>
+      <c r="L61" s="19"/>
       <c r="M61" s="16"/>
-      <c r="N61" s="30"/>
-      <c r="O61" s="30"/>
+      <c r="N61" s="42"/>
+      <c r="O61" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>

<commit_message>
27.06.19 Today sales details
</commit_message>
<xml_diff>
--- a/June/Others/Allocation Sheet.xlsx
+++ b/June/Others/Allocation Sheet.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="330" windowWidth="19875" windowHeight="7710"/>
+    <workbookView xWindow="360" yWindow="330" windowWidth="19875" windowHeight="7710" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Allocation Sheet" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="100">
   <si>
     <t>BL60</t>
   </si>
@@ -22,9 +23,6 @@
     <t>D22</t>
   </si>
   <si>
-    <t>B17</t>
-  </si>
-  <si>
     <t>BL90</t>
   </si>
   <si>
@@ -311,6 +309,12 @@
   </si>
   <si>
     <t>B60</t>
+  </si>
+  <si>
+    <t>B12+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               Total Qnt : </t>
   </si>
 </sst>
 </file>
@@ -320,7 +324,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +420,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -526,7 +538,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -598,14 +610,47 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -617,9 +662,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -636,26 +678,8 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -736,6 +760,187 @@
         <a:xfrm flipV="1">
           <a:off x="5753101" y="12614988"/>
           <a:ext cx="1514668" cy="2"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>29158</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>9719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38878</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>9720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Connector 1"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="29158" y="12230294"/>
+          <a:ext cx="2209995" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>194388</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9719</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>194390</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6819901" y="12224463"/>
+          <a:ext cx="1524193" cy="2"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>29158</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>9719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38878</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>9720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="29158" y="12230294"/>
+          <a:ext cx="2209995" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>194388</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9719</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>194390</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6819901" y="12224463"/>
+          <a:ext cx="1524193" cy="2"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1048,96 +1253,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N61" sqref="A1:O61"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="28" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="28"/>
-    <col min="3" max="4" width="8.140625" style="28" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="28" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="28" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="28" customWidth="1"/>
-    <col min="8" max="8" width="1.85546875" style="28" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="28" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="28" customWidth="1"/>
-    <col min="11" max="12" width="7.140625" style="28" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="28" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="28" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" style="28" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="28"/>
+    <col min="1" max="1" width="7.5703125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="27"/>
+    <col min="3" max="4" width="8.140625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="27" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" style="27" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="27" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" style="27" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="27" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="27" customWidth="1"/>
+    <col min="11" max="12" width="7.140625" style="27" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" style="27" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="27" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="27" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="32.25" customHeight="1">
-      <c r="A1" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
+      <c r="A1" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+    </row>
+    <row r="3" spans="1:18" s="28" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A3" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-    </row>
-    <row r="3" spans="1:18" s="29" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
     </row>
     <row r="4" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
+      <c r="A4" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
@@ -1145,61 +1350,61 @@
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
-      <c r="L4" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
+      <c r="L4" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickTop="1">
       <c r="A5" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="G5" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="O5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.95" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="6">
         <v>800</v>
@@ -1213,7 +1418,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J6" s="4">
         <v>4640</v>
@@ -1228,13 +1433,13 @@
     </row>
     <row r="7" spans="1:18" ht="15.95" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="B7" s="6">
-        <v>865</v>
+        <v>780</v>
       </c>
       <c r="C7" s="3">
-        <v>925</v>
+        <v>840</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1242,7 +1447,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J7" s="21">
         <v>5650</v>
@@ -1254,11 +1459,11 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="R7" s="30"/>
+      <c r="R7" s="29"/>
     </row>
     <row r="8" spans="1:18" ht="15.95" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="6">
         <v>810</v>
@@ -1272,7 +1477,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J8" s="2">
         <v>5020</v>
@@ -1287,7 +1492,7 @@
     </row>
     <row r="9" spans="1:18" ht="15.95" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="6">
         <v>800</v>
@@ -1301,7 +1506,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J9" s="4">
         <v>5280</v>
@@ -1316,7 +1521,7 @@
     </row>
     <row r="10" spans="1:18" ht="15.95" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="6">
         <v>795</v>
@@ -1330,7 +1535,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J10" s="4">
         <v>5100</v>
@@ -1345,7 +1550,7 @@
     </row>
     <row r="11" spans="1:18" ht="15.95" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="6">
         <v>790</v>
@@ -1359,7 +1564,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J11" s="4">
         <v>5560</v>
@@ -1374,7 +1579,7 @@
     </row>
     <row r="12" spans="1:18" ht="15.95" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="6">
         <v>800</v>
@@ -1388,7 +1593,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J12" s="4">
         <v>6090</v>
@@ -1403,7 +1608,7 @@
     </row>
     <row r="13" spans="1:18" ht="15.95" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="6">
         <v>970</v>
@@ -1417,7 +1622,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J13" s="4">
         <v>5390</v>
@@ -1432,7 +1637,7 @@
     </row>
     <row r="14" spans="1:18" ht="15.95" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="6">
         <v>900</v>
@@ -1446,7 +1651,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J14" s="4">
         <v>3630</v>
@@ -1475,7 +1680,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J15" s="4">
         <v>3560</v>
@@ -1490,7 +1695,7 @@
     </row>
     <row r="16" spans="1:18" ht="15.95" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="6">
         <v>910</v>
@@ -1504,7 +1709,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J16" s="4">
         <v>3340</v>
@@ -1519,7 +1724,7 @@
     </row>
     <row r="17" spans="1:15" ht="15.95" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="6">
         <v>890</v>
@@ -1533,7 +1738,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J17" s="4">
         <v>5390</v>
@@ -1548,7 +1753,7 @@
     </row>
     <row r="18" spans="1:15" ht="15.95" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" s="6">
         <v>920</v>
@@ -1562,7 +1767,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J18" s="4">
         <v>4500</v>
@@ -1577,7 +1782,7 @@
     </row>
     <row r="19" spans="1:15" ht="15.95" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="6">
         <v>880</v>
@@ -1591,7 +1796,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J19" s="4">
         <v>4970</v>
@@ -1606,7 +1811,7 @@
     </row>
     <row r="20" spans="1:15" ht="15.95" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="6">
         <v>1000</v>
@@ -1620,7 +1825,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J20" s="4">
         <v>4015</v>
@@ -1649,7 +1854,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J21" s="4">
         <v>3710</v>
@@ -1664,7 +1869,7 @@
     </row>
     <row r="22" spans="1:15" ht="15.95" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="6">
         <v>1000</v>
@@ -1678,7 +1883,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J22" s="4">
         <v>3620</v>
@@ -1693,7 +1898,7 @@
     </row>
     <row r="23" spans="1:15" ht="15.95" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="6">
         <v>960</v>
@@ -1707,7 +1912,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J23" s="4">
         <v>4620</v>
@@ -1722,7 +1927,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.95" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="6">
         <v>1040</v>
@@ -1736,7 +1941,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J24" s="4">
         <v>4520</v>
@@ -1751,7 +1956,7 @@
     </row>
     <row r="25" spans="1:15" ht="15.95" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="6">
         <v>1290</v>
@@ -1765,7 +1970,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J25" s="4">
         <v>4080</v>
@@ -1780,7 +1985,7 @@
     </row>
     <row r="26" spans="1:15" ht="15.95" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="6">
         <v>1190</v>
@@ -1794,7 +1999,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J26" s="4">
         <v>4220</v>
@@ -1809,7 +2014,7 @@
     </row>
     <row r="27" spans="1:15" ht="15.95" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" s="6">
         <v>1270</v>
@@ -1823,7 +2028,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J27" s="4">
         <v>12240</v>
@@ -1838,7 +2043,7 @@
     </row>
     <row r="28" spans="1:15" ht="15.95" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B28" s="6">
         <v>1170</v>
@@ -1852,7 +2057,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J28" s="4">
         <v>12090</v>
@@ -1867,7 +2072,7 @@
     </row>
     <row r="29" spans="1:15" ht="15.95" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" s="6">
         <v>1190</v>
@@ -1881,7 +2086,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J29" s="4">
         <v>10840</v>
@@ -1896,7 +2101,7 @@
     </row>
     <row r="30" spans="1:15" ht="15.95" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="6">
         <v>1225</v>
@@ -1910,7 +2115,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J30" s="21">
         <v>12490</v>
@@ -1925,7 +2130,7 @@
     </row>
     <row r="31" spans="1:15" ht="15.95" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="6">
         <v>1220</v>
@@ -1939,7 +2144,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J31" s="21">
         <v>8820</v>
@@ -1954,7 +2159,7 @@
     </row>
     <row r="32" spans="1:15" ht="15.95" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" s="6">
         <v>1080</v>
@@ -1977,7 +2182,7 @@
     </row>
     <row r="33" spans="1:15" ht="15.95" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="6">
         <v>1100</v>
@@ -2000,7 +2205,7 @@
     </row>
     <row r="34" spans="1:15" ht="15.95" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" s="6">
         <v>1200</v>
@@ -2023,7 +2228,7 @@
     </row>
     <row r="35" spans="1:15" ht="15.95" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B35" s="6">
         <v>1120</v>
@@ -2046,7 +2251,7 @@
     </row>
     <row r="36" spans="1:15" ht="15.95" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="7">
         <v>1040</v>
@@ -2069,7 +2274,7 @@
     </row>
     <row r="37" spans="1:15" ht="15.95" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" s="6">
         <v>1100</v>
@@ -2092,7 +2297,7 @@
     </row>
     <row r="38" spans="1:15" ht="15.95" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B38" s="6">
         <v>1100</v>
@@ -2115,7 +2320,7 @@
     </row>
     <row r="39" spans="1:15" ht="15.95" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B39" s="6">
         <v>1050</v>
@@ -2138,7 +2343,7 @@
     </row>
     <row r="40" spans="1:15" ht="15.95" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="6">
         <v>1130</v>
@@ -2161,7 +2366,7 @@
     </row>
     <row r="41" spans="1:15" ht="15.95" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B41" s="6">
         <v>1100</v>
@@ -2184,7 +2389,7 @@
     </row>
     <row r="42" spans="1:15" ht="15.95" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="6">
         <v>1330</v>
@@ -2207,7 +2412,7 @@
     </row>
     <row r="43" spans="1:15" ht="15.95" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B43" s="6">
         <v>1200</v>
@@ -2230,7 +2435,7 @@
     </row>
     <row r="44" spans="1:15" ht="15.95" customHeight="1">
       <c r="A44" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" s="6">
         <v>1250</v>
@@ -2243,19 +2448,19 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="I44" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="J44" s="36"/>
+      <c r="I44" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="J44" s="46"/>
       <c r="K44" s="22"/>
       <c r="L44" s="22"/>
-      <c r="M44" s="35"/>
-      <c r="N44" s="35"/>
+      <c r="M44" s="36"/>
+      <c r="N44" s="36"/>
       <c r="O44" s="12"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="6">
         <v>1370</v>
@@ -2268,17 +2473,17 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
-      <c r="K45" s="35"/>
-      <c r="L45" s="35"/>
-      <c r="M45" s="35"/>
-      <c r="N45" s="35"/>
-      <c r="O45" s="35"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="36"/>
+      <c r="L45" s="36"/>
+      <c r="M45" s="36"/>
+      <c r="N45" s="36"/>
+      <c r="O45" s="36"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B46" s="6">
         <v>2780</v>
@@ -2291,19 +2496,19 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-      <c r="I46" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="J46" s="43"/>
-      <c r="K46" s="43"/>
-      <c r="L46" s="43"/>
-      <c r="M46" s="43"/>
-      <c r="N46" s="43"/>
-      <c r="O46" s="44"/>
+      <c r="I46" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="J46" s="37"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
+      <c r="M46" s="37"/>
+      <c r="N46" s="37"/>
+      <c r="O46" s="38"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B47" s="6">
         <v>6540</v>
@@ -2317,22 +2522,22 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J47" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K47" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="K47" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="L47" s="47"/>
-      <c r="M47" s="47"/>
-      <c r="N47" s="47"/>
-      <c r="O47" s="45"/>
+      <c r="L47" s="41"/>
+      <c r="M47" s="41"/>
+      <c r="N47" s="41"/>
+      <c r="O47" s="39"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B48" s="6">
         <v>5290</v>
@@ -2353,11 +2558,11 @@
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
-      <c r="O48" s="45"/>
+      <c r="O48" s="39"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B49" s="6">
         <v>5470</v>
@@ -2378,11 +2583,11 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
-      <c r="O49" s="45"/>
+      <c r="O49" s="39"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B50" s="3">
         <v>5750</v>
@@ -2403,11 +2608,11 @@
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
-      <c r="O50" s="45"/>
+      <c r="O50" s="39"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B51" s="3">
         <v>5940</v>
@@ -2428,11 +2633,11 @@
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
-      <c r="O51" s="45"/>
+      <c r="O51" s="39"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="3">
         <v>6530</v>
@@ -2453,11 +2658,11 @@
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
-      <c r="O52" s="45"/>
+      <c r="O52" s="39"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B53" s="3">
         <v>8340</v>
@@ -2478,11 +2683,11 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
-      <c r="O53" s="45"/>
+      <c r="O53" s="39"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B54" s="3">
         <v>9190</v>
@@ -2503,11 +2708,11 @@
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
-      <c r="O54" s="45"/>
+      <c r="O54" s="39"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B55" s="3">
         <v>5750</v>
@@ -2528,11 +2733,11 @@
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
-      <c r="O55" s="45"/>
+      <c r="O55" s="39"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B56" s="2">
         <v>5570</v>
@@ -2546,14 +2751,14 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
-      <c r="O56" s="46"/>
+      <c r="O56" s="40"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="11"/>
@@ -2573,47 +2778,49 @@
       <c r="O57" s="24"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="B58" s="41"/>
-      <c r="C58" s="41"/>
+      <c r="A58" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
       <c r="D58" s="19"/>
       <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
-      <c r="I58" s="25"/>
-      <c r="J58" s="26"/>
-      <c r="K58" s="19"/>
+      <c r="F58" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="G58" s="51"/>
+      <c r="H58" s="51"/>
+      <c r="I58" s="51"/>
+      <c r="J58" s="51"/>
+      <c r="K58" s="51"/>
       <c r="L58" s="19"/>
       <c r="M58" s="25"/>
-      <c r="N58" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="O58" s="42"/>
+      <c r="N58" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="O58" s="35"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="34"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="34"/>
+      <c r="A59" s="45"/>
+      <c r="B59" s="45"/>
+      <c r="C59" s="45"/>
       <c r="D59" s="18"/>
       <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="23"/>
-      <c r="K59" s="18"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="51"/>
+      <c r="H59" s="51"/>
+      <c r="I59" s="51"/>
+      <c r="J59" s="51"/>
+      <c r="K59" s="51"/>
       <c r="L59" s="18"/>
       <c r="M59" s="11"/>
-      <c r="N59" s="34"/>
-      <c r="O59" s="34"/>
+      <c r="N59" s="45"/>
+      <c r="O59" s="45"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="34"/>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
+      <c r="A60" s="45"/>
+      <c r="B60" s="45"/>
+      <c r="C60" s="45"/>
       <c r="D60" s="18"/>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
@@ -2624,38 +2831,30 @@
       <c r="K60" s="18"/>
       <c r="L60" s="18"/>
       <c r="M60" s="11"/>
-      <c r="N60" s="34"/>
-      <c r="O60" s="34"/>
+      <c r="N60" s="45"/>
+      <c r="O60" s="45"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B61" s="41"/>
-      <c r="C61" s="41"/>
+      <c r="A61" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="34"/>
+      <c r="C61" s="34"/>
       <c r="D61" s="19"/>
       <c r="E61" s="19"/>
       <c r="F61" s="19"/>
       <c r="G61" s="19"/>
       <c r="H61" s="19"/>
       <c r="I61" s="19"/>
-      <c r="J61" s="27"/>
+      <c r="J61" s="26"/>
       <c r="K61" s="19"/>
       <c r="L61" s="19"/>
       <c r="M61" s="16"/>
-      <c r="N61" s="42"/>
-      <c r="O61" s="42"/>
+      <c r="N61" s="35"/>
+      <c r="O61" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="N58:O58"/>
+  <mergeCells count="20">
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="A1:E1"/>
@@ -2667,10 +2866,1634 @@
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="A4:D4"/>
+    <mergeCell ref="F58:K59"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="N58:O58"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="80" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="42.75">
+      <c r="A1" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+    </row>
+    <row r="4" spans="1:15" ht="16.5" thickBot="1">
+      <c r="A4" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" thickTop="1">
+      <c r="A5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="6">
+        <v>800</v>
+      </c>
+      <c r="C6" s="3">
+        <v>875</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6" s="4">
+        <v>4640</v>
+      </c>
+      <c r="K6" s="3">
+        <v>4990</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="6">
+        <v>780</v>
+      </c>
+      <c r="C7" s="3">
+        <v>840</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="21">
+        <v>5650</v>
+      </c>
+      <c r="K7" s="3">
+        <v>6150</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="6">
+        <v>810</v>
+      </c>
+      <c r="C8" s="3">
+        <v>880</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5020</v>
+      </c>
+      <c r="K8" s="3">
+        <v>5390</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="6">
+        <v>800</v>
+      </c>
+      <c r="C9" s="3">
+        <v>870</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="4">
+        <v>5280</v>
+      </c>
+      <c r="K9" s="3">
+        <v>5690</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="6">
+        <v>795</v>
+      </c>
+      <c r="C10" s="3">
+        <v>865</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" s="4">
+        <v>5100</v>
+      </c>
+      <c r="K10" s="3">
+        <v>5490</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="6">
+        <v>790</v>
+      </c>
+      <c r="C11" s="3">
+        <v>860</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="4">
+        <v>5560</v>
+      </c>
+      <c r="K11" s="3">
+        <v>5990</v>
+      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="6">
+        <v>800</v>
+      </c>
+      <c r="C12" s="3">
+        <v>860</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="4">
+        <v>6090</v>
+      </c>
+      <c r="K12" s="3">
+        <v>6590</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="6">
+        <v>970</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1060</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="4">
+        <v>5390</v>
+      </c>
+      <c r="K13" s="3">
+        <v>5790</v>
+      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="6">
+        <v>900</v>
+      </c>
+      <c r="C14" s="3">
+        <v>975</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="4">
+        <v>3630</v>
+      </c>
+      <c r="K14" s="3">
+        <v>3890</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="6">
+        <v>915</v>
+      </c>
+      <c r="C15" s="3">
+        <v>990</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="4">
+        <v>3560</v>
+      </c>
+      <c r="K15" s="3">
+        <v>3840</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="6">
+        <v>910</v>
+      </c>
+      <c r="C16" s="3">
+        <v>980</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J16" s="4">
+        <v>3340</v>
+      </c>
+      <c r="K16" s="3">
+        <v>3590</v>
+      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6">
+        <v>890</v>
+      </c>
+      <c r="C17" s="3">
+        <v>970</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" s="4">
+        <v>5390</v>
+      </c>
+      <c r="K17" s="3">
+        <v>5790</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="6">
+        <v>920</v>
+      </c>
+      <c r="C18" s="3">
+        <v>999</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J18" s="4">
+        <v>4500</v>
+      </c>
+      <c r="K18" s="3">
+        <v>4790</v>
+      </c>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="6">
+        <v>880</v>
+      </c>
+      <c r="C19" s="3">
+        <v>950</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="4">
+        <v>4970</v>
+      </c>
+      <c r="K19" s="3">
+        <v>5290</v>
+      </c>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1000</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1090</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" s="4">
+        <v>4015</v>
+      </c>
+      <c r="K20" s="3">
+        <v>4390</v>
+      </c>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="6">
+        <v>995</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1075</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="4">
+        <v>3710</v>
+      </c>
+      <c r="K21" s="3">
+        <v>3990</v>
+      </c>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="6">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1090</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J22" s="4">
+        <v>3620</v>
+      </c>
+      <c r="K22" s="3">
+        <v>3890</v>
+      </c>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="6">
+        <v>960</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1040</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="4">
+        <v>4620</v>
+      </c>
+      <c r="K23" s="3">
+        <v>4999</v>
+      </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="6">
+        <v>1040</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1120</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="4">
+        <v>4520</v>
+      </c>
+      <c r="K24" s="3">
+        <v>4899</v>
+      </c>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="6">
+        <v>1290</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1390</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J25" s="4">
+        <v>4080</v>
+      </c>
+      <c r="K25" s="3">
+        <v>4390</v>
+      </c>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1190</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1290</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J26" s="4">
+        <v>4220</v>
+      </c>
+      <c r="K26" s="3">
+        <v>4540</v>
+      </c>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="6">
+        <v>1270</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1370</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" s="4">
+        <v>12240</v>
+      </c>
+      <c r="K27" s="3">
+        <v>12990</v>
+      </c>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="6">
+        <v>1170</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1270</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="J28" s="4">
+        <v>12090</v>
+      </c>
+      <c r="K28" s="3">
+        <v>12990</v>
+      </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="6">
+        <v>1190</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1290</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="J29" s="4">
+        <v>10840</v>
+      </c>
+      <c r="K29" s="3">
+        <v>11990</v>
+      </c>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="6">
+        <v>1225</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1325</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J30" s="21">
+        <v>12490</v>
+      </c>
+      <c r="K30" s="3">
+        <v>13490</v>
+      </c>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="6">
+        <v>1220</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1320</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="J31" s="21">
+        <v>8820</v>
+      </c>
+      <c r="K31" s="3">
+        <v>9490</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="6">
+        <v>1080</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1160</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="6">
+        <v>1100</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1199</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="6">
+        <v>1200</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1290</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="6">
+        <v>1120</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1220</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="7">
+        <v>1040</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1130</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="6">
+        <v>1100</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1199</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="6">
+        <v>1100</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1199</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="6">
+        <v>1050</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1130</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="6">
+        <v>1130</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1230</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="6">
+        <v>1100</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1190</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="6">
+        <v>1330</v>
+      </c>
+      <c r="C42" s="3">
+        <v>1450</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="6">
+        <v>1200</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1299</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+    </row>
+    <row r="44" spans="1:15" ht="15.75">
+      <c r="A44" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="6">
+        <v>1250</v>
+      </c>
+      <c r="C44" s="3">
+        <v>1350</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="J44" s="46"/>
+      <c r="K44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="36"/>
+      <c r="N44" s="36"/>
+      <c r="O44" s="12"/>
+    </row>
+    <row r="45" spans="1:15" ht="15.75">
+      <c r="A45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="6">
+        <v>1370</v>
+      </c>
+      <c r="C45" s="3">
+        <v>1490</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="36"/>
+      <c r="L45" s="36"/>
+      <c r="M45" s="36"/>
+      <c r="N45" s="36"/>
+      <c r="O45" s="36"/>
+    </row>
+    <row r="46" spans="1:15" ht="15.75">
+      <c r="A46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="6">
+        <v>2780</v>
+      </c>
+      <c r="C46" s="3">
+        <v>2990</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="J46" s="37"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
+      <c r="M46" s="37"/>
+      <c r="N46" s="37"/>
+      <c r="O46" s="38"/>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" s="6">
+        <v>6540</v>
+      </c>
+      <c r="C47" s="3">
+        <v>6990</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K47" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="L47" s="41"/>
+      <c r="M47" s="41"/>
+      <c r="N47" s="41"/>
+      <c r="O47" s="39"/>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="6">
+        <v>5290</v>
+      </c>
+      <c r="C48" s="3">
+        <v>5690</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="33">
+        <v>1000</v>
+      </c>
+      <c r="J48" s="5"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="39"/>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" s="6">
+        <v>5470</v>
+      </c>
+      <c r="C49" s="3">
+        <v>5890</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="33">
+        <v>500</v>
+      </c>
+      <c r="J49" s="5"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="39"/>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="3">
+        <v>5750</v>
+      </c>
+      <c r="C50" s="3">
+        <v>6190</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="33">
+        <v>100</v>
+      </c>
+      <c r="J50" s="5"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="39"/>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="3">
+        <v>5940</v>
+      </c>
+      <c r="C51" s="3">
+        <v>6390</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="33">
+        <v>50</v>
+      </c>
+      <c r="J51" s="5"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="39"/>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="3">
+        <v>6530</v>
+      </c>
+      <c r="C52" s="3">
+        <v>6990</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="33">
+        <v>20</v>
+      </c>
+      <c r="J52" s="5"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="39"/>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="3">
+        <v>8340</v>
+      </c>
+      <c r="C53" s="3">
+        <v>8990</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="33">
+        <v>10</v>
+      </c>
+      <c r="J53" s="5"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="39"/>
+    </row>
+    <row r="54" spans="1:15">
+      <c r="A54" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" s="3">
+        <v>9190</v>
+      </c>
+      <c r="C54" s="3">
+        <v>9990</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="33">
+        <v>5</v>
+      </c>
+      <c r="J54" s="5"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="39"/>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="3">
+        <v>5750</v>
+      </c>
+      <c r="C55" s="3">
+        <v>6190</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="33">
+        <v>2</v>
+      </c>
+      <c r="J55" s="5"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="39"/>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="2">
+        <v>5570</v>
+      </c>
+      <c r="C56" s="2">
+        <v>5990</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="40"/>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" s="11"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="23"/>
+      <c r="K57" s="30"/>
+      <c r="L57" s="30"/>
+      <c r="M57" s="24"/>
+      <c r="N57" s="24"/>
+      <c r="O57" s="24"/>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="G58" s="51"/>
+      <c r="H58" s="51"/>
+      <c r="I58" s="51"/>
+      <c r="J58" s="51"/>
+      <c r="K58" s="51"/>
+      <c r="L58" s="32"/>
+      <c r="M58" s="25"/>
+      <c r="N58" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="O58" s="35"/>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="A59" s="45"/>
+      <c r="B59" s="45"/>
+      <c r="C59" s="45"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="51"/>
+      <c r="H59" s="51"/>
+      <c r="I59" s="51"/>
+      <c r="J59" s="51"/>
+      <c r="K59" s="51"/>
+      <c r="L59" s="30"/>
+      <c r="M59" s="11"/>
+      <c r="N59" s="45"/>
+      <c r="O59" s="45"/>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="A60" s="45"/>
+      <c r="B60" s="45"/>
+      <c r="C60" s="45"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="23"/>
+      <c r="K60" s="30"/>
+      <c r="L60" s="30"/>
+      <c r="M60" s="11"/>
+      <c r="N60" s="45"/>
+      <c r="O60" s="45"/>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="A61" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="34"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="32"/>
+      <c r="I61" s="32"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="32"/>
+      <c r="L61" s="32"/>
+      <c r="M61" s="16"/>
+      <c r="N61" s="35"/>
+      <c r="O61" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="A59:C60"/>
+    <mergeCell ref="N59:O60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="F58:K59"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L4:O4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>